<commit_message>
Latest excel file - v3
</commit_message>
<xml_diff>
--- a/Summary of Files.xlsx
+++ b/Summary of Files.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10227" uniqueCount="2200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10270" uniqueCount="2201">
   <si>
     <t>Folder</t>
   </si>
@@ -6627,6 +6627,9 @@
   </si>
   <si>
     <t>N/A - Report</t>
+  </si>
+  <si>
+    <t>Not Usable - Levi9 Overall</t>
   </si>
 </sst>
 </file>
@@ -6665,10 +6668,12 @@
       <b/>
       <sz val="10"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -7072,12 +7077,12 @@
   <dimension ref="A1:JY326"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.140625" customWidth="1"/>
     <col min="4" max="4" width="38.140625" bestFit="1" customWidth="1"/>
@@ -8479,6 +8484,9 @@
       </c>
     </row>
     <row r="11" spans="1:285" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B11" s="10" t="s">
         <v>273</v>
       </c>
@@ -8913,6 +8921,9 @@
       </c>
     </row>
     <row r="12" spans="1:285" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B12" s="10" t="s">
         <v>273</v>
       </c>
@@ -8978,6 +8989,9 @@
       </c>
     </row>
     <row r="13" spans="1:285" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B13" s="10" t="s">
         <v>273</v>
       </c>
@@ -9134,6 +9148,9 @@
       </c>
     </row>
     <row r="16" spans="1:285" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B16" s="10" t="s">
         <v>273</v>
       </c>
@@ -9290,6 +9307,9 @@
       </c>
     </row>
     <row r="19" spans="1:75" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B19" s="10" t="s">
         <v>273</v>
       </c>
@@ -9455,6 +9475,9 @@
       </c>
     </row>
     <row r="22" spans="1:75" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B22" s="10" t="s">
         <v>273</v>
       </c>
@@ -9620,6 +9643,9 @@
       </c>
     </row>
     <row r="25" spans="1:75" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B25" s="10" t="s">
         <v>273</v>
       </c>
@@ -9740,6 +9766,9 @@
       </c>
     </row>
     <row r="28" spans="1:75" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B28" s="10" t="s">
         <v>273</v>
       </c>
@@ -9826,6 +9855,9 @@
       </c>
     </row>
     <row r="29" spans="1:75" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B29" s="10" t="s">
         <v>273</v>
       </c>
@@ -10023,6 +10055,9 @@
       </c>
     </row>
     <row r="30" spans="1:75" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B30" s="10" t="s">
         <v>273</v>
       </c>
@@ -10247,6 +10282,9 @@
       </c>
     </row>
     <row r="31" spans="1:75" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B31" s="10" t="s">
         <v>273</v>
       </c>
@@ -11445,6 +11483,9 @@
       </c>
     </row>
     <row r="36" spans="1:263" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B36" s="10" t="s">
         <v>273</v>
       </c>
@@ -11667,6 +11708,9 @@
       </c>
     </row>
     <row r="39" spans="1:263" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B39" s="10" t="s">
         <v>273</v>
       </c>
@@ -12078,6 +12122,9 @@
       </c>
     </row>
     <row r="42" spans="1:263" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B42" s="10" t="s">
         <v>273</v>
       </c>
@@ -13959,6 +14006,9 @@
       </c>
     </row>
     <row r="45" spans="1:263" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B45" s="10" t="s">
         <v>273</v>
       </c>
@@ -14277,6 +14327,9 @@
       </c>
     </row>
     <row r="48" spans="1:263" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B48" s="10" t="s">
         <v>273</v>
       </c>
@@ -14357,6 +14410,9 @@
       </c>
     </row>
     <row r="49" spans="1:42" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B49" s="10" t="s">
         <v>273</v>
       </c>
@@ -14482,6 +14538,9 @@
       </c>
     </row>
     <row r="50" spans="1:42" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B50" s="10" t="s">
         <v>273</v>
       </c>
@@ -14611,6 +14670,9 @@
       </c>
     </row>
     <row r="53" spans="1:42" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B53" s="10" t="s">
         <v>273</v>
       </c>
@@ -14740,6 +14802,9 @@
       </c>
     </row>
     <row r="56" spans="1:42" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B56" s="10" t="s">
         <v>273</v>
       </c>
@@ -14769,6 +14834,9 @@
       </c>
     </row>
     <row r="57" spans="1:42" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B57" s="10" t="s">
         <v>273</v>
       </c>
@@ -14798,6 +14866,9 @@
       </c>
     </row>
     <row r="58" spans="1:42" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B58" s="10" t="s">
         <v>273</v>
       </c>
@@ -14827,6 +14898,9 @@
       </c>
     </row>
     <row r="59" spans="1:42" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B59" s="10" t="s">
         <v>273</v>
       </c>
@@ -14856,6 +14930,9 @@
       </c>
     </row>
     <row r="60" spans="1:42" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B60" s="10" t="s">
         <v>273</v>
       </c>
@@ -14885,6 +14962,9 @@
       </c>
     </row>
     <row r="61" spans="1:42" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B61" s="10" t="s">
         <v>273</v>
       </c>
@@ -14914,6 +14994,9 @@
       </c>
     </row>
     <row r="62" spans="1:42" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B62" s="10" t="s">
         <v>273</v>
       </c>
@@ -14943,6 +15026,9 @@
       </c>
     </row>
     <row r="63" spans="1:42" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B63" s="10" t="s">
         <v>273</v>
       </c>
@@ -14972,6 +15058,9 @@
       </c>
     </row>
     <row r="64" spans="1:42" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B64" s="10" t="s">
         <v>273</v>
       </c>
@@ -15110,6 +15199,9 @@
       </c>
     </row>
     <row r="67" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B67" s="10" t="s">
         <v>273</v>
       </c>
@@ -15248,6 +15340,9 @@
       </c>
     </row>
     <row r="70" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B70" s="10" t="s">
         <v>273</v>
       </c>
@@ -15346,6 +15441,9 @@
       </c>
     </row>
     <row r="71" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B71" s="10" t="s">
         <v>273</v>
       </c>
@@ -15425,6 +15523,9 @@
       </c>
     </row>
     <row r="73" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B73" s="10" t="s">
         <v>273</v>
       </c>
@@ -15504,6 +15605,9 @@
       </c>
     </row>
     <row r="75" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B75" s="10" t="s">
         <v>273</v>
       </c>
@@ -15583,6 +15687,9 @@
       </c>
     </row>
     <row r="77" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B77" s="10" t="s">
         <v>273</v>
       </c>
@@ -15800,6 +15907,9 @@
       </c>
     </row>
     <row r="79" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B79" s="10" t="s">
         <v>273</v>
       </c>
@@ -16017,6 +16127,9 @@
       </c>
     </row>
     <row r="81" spans="1:146" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B81" s="10" t="s">
         <v>273</v>
       </c>
@@ -38353,6 +38466,9 @@
       </c>
     </row>
     <row r="299" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A299" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B299" s="10" t="s">
         <v>273</v>
       </c>
@@ -38472,6 +38588,9 @@
       </c>
     </row>
     <row r="300" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A300" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B300" s="10" t="s">
         <v>273</v>
       </c>
@@ -38528,6 +38647,9 @@
       </c>
     </row>
     <row r="301" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A301" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B301" s="10" t="s">
         <v>273</v>
       </c>
@@ -38584,6 +38706,9 @@
       </c>
     </row>
     <row r="302" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A302" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B302" s="10" t="s">
         <v>273</v>
       </c>
@@ -38643,6 +38768,9 @@
       </c>
     </row>
     <row r="303" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A303" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B303" s="10" t="s">
         <v>273</v>
       </c>
@@ -38702,6 +38830,9 @@
       </c>
     </row>
     <row r="304" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A304" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B304" s="10" t="s">
         <v>273</v>
       </c>
@@ -38754,7 +38885,10 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="305" spans="2:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A305" s="10" t="s">
+        <v>2200</v>
+      </c>
       <c r="B305" s="10" t="s">
         <v>273</v>
       </c>
@@ -38807,7 +38941,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="306" spans="2:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B306" s="10" t="s">
         <v>273</v>
       </c>
@@ -38926,7 +39060,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="307" spans="2:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B307" s="10" t="s">
         <v>273</v>
       </c>
@@ -38982,7 +39116,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="308" spans="2:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B308" s="10" t="s">
         <v>273</v>
       </c>
@@ -39038,7 +39172,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="309" spans="2:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B309" s="10" t="s">
         <v>273</v>
       </c>
@@ -39097,7 +39231,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="310" spans="2:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B310" s="10" t="s">
         <v>273</v>
       </c>
@@ -39156,7 +39290,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="311" spans="2:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B311" s="10" t="s">
         <v>273</v>
       </c>
@@ -39209,7 +39343,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="312" spans="2:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B312" s="10" t="s">
         <v>273</v>
       </c>
@@ -39262,7 +39396,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="313" spans="2:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B313" s="10" t="s">
         <v>273</v>
       </c>
@@ -39381,7 +39515,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="314" spans="2:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B314" s="10" t="s">
         <v>273</v>
       </c>
@@ -39437,7 +39571,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="315" spans="2:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B315" s="10" t="s">
         <v>273</v>
       </c>
@@ -39493,7 +39627,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="316" spans="2:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B316" s="10" t="s">
         <v>273</v>
       </c>
@@ -39552,7 +39686,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="317" spans="2:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B317" s="10" t="s">
         <v>273</v>
       </c>
@@ -39611,7 +39745,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="318" spans="2:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B318" s="10" t="s">
         <v>273</v>
       </c>
@@ -39664,7 +39798,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="319" spans="2:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B319" s="10" t="s">
         <v>273</v>
       </c>
@@ -39717,7 +39851,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="320" spans="2:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:41" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B320" s="10" t="s">
         <v>273</v>
       </c>

</xml_diff>

<commit_message>
updated Reporting Team Feedback - v4
</commit_message>
<xml_diff>
--- a/Summary of Files.xlsx
+++ b/Summary of Files.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10270" uniqueCount="2201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10294" uniqueCount="2202">
   <si>
     <t>Folder</t>
   </si>
@@ -6630,6 +6630,9 @@
   </si>
   <si>
     <t>Not Usable - Levi9 Overall</t>
+  </si>
+  <si>
+    <t>No Data</t>
   </si>
 </sst>
 </file>
@@ -7077,7 +7080,7 @@
   <dimension ref="A1:JY326"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21912,6 +21915,9 @@
       </c>
     </row>
     <row r="128" spans="1:173" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="10" t="s">
+        <v>2201</v>
+      </c>
       <c r="B128" s="10" t="s">
         <v>273</v>
       </c>
@@ -21941,6 +21947,9 @@
       </c>
     </row>
     <row r="129" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="10" t="s">
+        <v>2201</v>
+      </c>
       <c r="B129" s="10" t="s">
         <v>273</v>
       </c>
@@ -21970,6 +21979,9 @@
       </c>
     </row>
     <row r="130" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="10" t="s">
+        <v>2201</v>
+      </c>
       <c r="B130" s="10" t="s">
         <v>273</v>
       </c>
@@ -21999,6 +22011,9 @@
       </c>
     </row>
     <row r="131" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="10" t="s">
+        <v>2201</v>
+      </c>
       <c r="B131" s="10" t="s">
         <v>273</v>
       </c>
@@ -22028,6 +22043,9 @@
       </c>
     </row>
     <row r="132" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="10" t="s">
+        <v>2201</v>
+      </c>
       <c r="B132" s="10" t="s">
         <v>273</v>
       </c>
@@ -22057,6 +22075,9 @@
       </c>
     </row>
     <row r="133" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="10" t="s">
+        <v>2201</v>
+      </c>
       <c r="B133" s="10" t="s">
         <v>273</v>
       </c>
@@ -22086,6 +22107,9 @@
       </c>
     </row>
     <row r="134" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="10" t="s">
+        <v>2201</v>
+      </c>
       <c r="B134" s="10" t="s">
         <v>273</v>
       </c>
@@ -22115,6 +22139,9 @@
       </c>
     </row>
     <row r="135" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="10" t="s">
+        <v>2201</v>
+      </c>
       <c r="B135" s="10" t="s">
         <v>273</v>
       </c>
@@ -29166,6 +29193,9 @@
       </c>
     </row>
     <row r="200" spans="1:62" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A200" s="10" t="s">
+        <v>2201</v>
+      </c>
       <c r="B200" s="10" t="s">
         <v>273</v>
       </c>
@@ -29195,6 +29225,9 @@
       </c>
     </row>
     <row r="201" spans="1:62" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A201" s="10" t="s">
+        <v>2201</v>
+      </c>
       <c r="B201" s="10" t="s">
         <v>273</v>
       </c>
@@ -29224,6 +29257,9 @@
       </c>
     </row>
     <row r="202" spans="1:62" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A202" s="10" t="s">
+        <v>2201</v>
+      </c>
       <c r="B202" s="10" t="s">
         <v>273</v>
       </c>
@@ -29253,6 +29289,9 @@
       </c>
     </row>
     <row r="203" spans="1:62" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A203" s="10" t="s">
+        <v>2201</v>
+      </c>
       <c r="B203" s="10" t="s">
         <v>273</v>
       </c>
@@ -29282,6 +29321,9 @@
       </c>
     </row>
     <row r="204" spans="1:62" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A204" s="10" t="s">
+        <v>2201</v>
+      </c>
       <c r="B204" s="10" t="s">
         <v>273</v>
       </c>
@@ -29311,6 +29353,9 @@
       </c>
     </row>
     <row r="205" spans="1:62" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A205" s="10" t="s">
+        <v>2201</v>
+      </c>
       <c r="B205" s="10" t="s">
         <v>273</v>
       </c>
@@ -29340,6 +29385,9 @@
       </c>
     </row>
     <row r="206" spans="1:62" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A206" s="10" t="s">
+        <v>2201</v>
+      </c>
       <c r="B206" s="10" t="s">
         <v>273</v>
       </c>
@@ -29369,6 +29417,9 @@
       </c>
     </row>
     <row r="207" spans="1:62" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A207" s="10" t="s">
+        <v>2201</v>
+      </c>
       <c r="B207" s="10" t="s">
         <v>273</v>
       </c>
@@ -36972,6 +37023,9 @@
       </c>
     </row>
     <row r="272" spans="1:226" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A272" s="10" t="s">
+        <v>2201</v>
+      </c>
       <c r="B272" s="10" t="s">
         <v>273</v>
       </c>
@@ -37001,6 +37055,9 @@
       </c>
     </row>
     <row r="273" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A273" s="10" t="s">
+        <v>2201</v>
+      </c>
       <c r="B273" s="10" t="s">
         <v>273</v>
       </c>
@@ -37030,6 +37087,9 @@
       </c>
     </row>
     <row r="274" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A274" s="10" t="s">
+        <v>2201</v>
+      </c>
       <c r="B274" s="10" t="s">
         <v>273</v>
       </c>
@@ -37059,6 +37119,9 @@
       </c>
     </row>
     <row r="275" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A275" s="10" t="s">
+        <v>2201</v>
+      </c>
       <c r="B275" s="10" t="s">
         <v>273</v>
       </c>
@@ -37088,6 +37151,9 @@
       </c>
     </row>
     <row r="276" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A276" s="10" t="s">
+        <v>2201</v>
+      </c>
       <c r="B276" s="10" t="s">
         <v>273</v>
       </c>
@@ -37117,6 +37183,9 @@
       </c>
     </row>
     <row r="277" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A277" s="10" t="s">
+        <v>2201</v>
+      </c>
       <c r="B277" s="10" t="s">
         <v>273</v>
       </c>
@@ -37146,6 +37215,9 @@
       </c>
     </row>
     <row r="278" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A278" s="10" t="s">
+        <v>2201</v>
+      </c>
       <c r="B278" s="10" t="s">
         <v>273</v>
       </c>
@@ -37175,6 +37247,9 @@
       </c>
     </row>
     <row r="279" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A279" s="10" t="s">
+        <v>2201</v>
+      </c>
       <c r="B279" s="10" t="s">
         <v>273</v>
       </c>

</xml_diff>